<commit_message>
update limit hutang dan dikirim via
</commit_message>
<xml_diff>
--- a/storage/exports/client-form-format.xlsx
+++ b/storage/exports/client-form-format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit</t>
   </si>
   <si>
     <t xml:space="preserve">Mobile</t>
@@ -269,26 +272,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:R2"/>
+  <dimension ref="A2:S2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="46.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="16" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true" ht="16.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -322,7 +325,7 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -343,14 +346,17 @@
       <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -365,18 +371,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A3:C3 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -391,18 +397,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A3:C3 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
update SO packaging and export
</commit_message>
<xml_diff>
--- a/storage/exports/client-form-format.xlsx
+++ b/storage/exports/client-form-format.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Label</t>
   </si>
   <si>
     <t xml:space="preserve">Mobile</t>
@@ -272,29 +275,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:S2"/>
+  <dimension ref="A2:T2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.0102040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="17" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true" ht="16.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -331,7 +334,7 @@
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -352,8 +355,11 @@
       <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -380,7 +386,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -406,7 +412,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update SO and Client
</commit_message>
<xml_diff>
--- a/storage/exports/client-form-format.xlsx
+++ b/storage/exports/client-form-format.xlsx
@@ -275,28 +275,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:T2"/>
+  <dimension ref="2:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.05102040816327"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0918367346939"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3520408163265"/>
     <col collapsed="false" hidden="false" max="17" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="41.7142857142857"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
@@ -361,6 +361,7 @@
       <c r="T2" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>